<commit_message>
[finishes #183800220] Practice Quizzes are uploaded.
</commit_message>
<xml_diff>
--- a/planning/questions/questions-earth_sci.xlsx
+++ b/planning/questions/questions-earth_sci.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GBDSFC03\Documents\GitHub\capstone_ScienceClubWebsite\planning\questions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67E9D369-64FE-49A7-9676-C80BD624870A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0234D132-7729-4748-962B-A9E95A3B8816}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Astronomy" sheetId="2" r:id="rId1"/>
@@ -18,17 +18,28 @@
     <sheet name="Remote_Sensing" sheetId="3" r:id="rId3"/>
     <sheet name="Template" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="66">
   <si>
     <t>Question</t>
   </si>
@@ -223,6 +234,9 @@
   </si>
   <si>
     <t>Rough surface</t>
+  </si>
+  <si>
+    <t>Question Concatenated</t>
   </si>
 </sst>
 </file>
@@ -580,21 +594,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B06BFF7-08AB-4875-A27F-CD885511EC6D}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:C1048576"/>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="12"/>
-    <col min="2" max="2" width="69.88671875" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42.77734375" style="4" customWidth="1"/>
+    <col min="2" max="4" width="35.33203125" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
         <v>2</v>
       </c>
@@ -602,179 +615,262 @@
         <v>0</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="12">
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="4" t="str">
+        <f>_xlfn.CONCAT(A2,". ",B2)</f>
+        <v>1. What percentage of the mass-energy of the universe is made up of dark energy?</v>
+      </c>
+      <c r="D2" s="5">
         <v>0.68</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="12">
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="4" t="str">
+        <f t="shared" ref="C3:C21" si="0">_xlfn.CONCAT(A3,". ",B3)</f>
+        <v>2. Quantom Field Theory predicts the value of the cosmological constant to be _____ orders of magnitude larger than we observe.</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="12">
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>3. How are galaxies organized and distributed within the universe?</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A5" s="12">
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>4. What would an outside observer see as an object approaches and crosses the event horizon of a black hole?</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="12">
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>5. What relationship relates the luminosity of a galaxy to its rotational speed?</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="12">
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>6. What is the average temperature of the Cosmic Microwave Background?</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="12">
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>7. About what percent of the universe’s baryons are believed to exist in the Warm-Hot Intergalactic Medium?</v>
+      </c>
+      <c r="D8" s="5">
         <v>0.4</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="12">
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>8. Which stars are younger and more luminous?</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="12">
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>9. Which stellar population is more common in globular clusters?</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="12">
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>10. The motion of the Andromeda galaxy towards the Milky Way galaxy despite the overall expansion of space is an example of which of the following?</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="12">
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>11. Which of the following characterizes a starburst galaxy?</v>
+      </c>
+      <c r="D12" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="72" x14ac:dyDescent="0.3">
       <c r="A13" s="12">
         <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>12. The No Hair theorem states that a black hole can be completely characterized by three externally observable characteristics. What are these three characteristics?</v>
+      </c>
+      <c r="D13" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="12">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C14" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">13. </v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="12">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C15" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">14. </v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="12">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C16" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">15. </v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="12">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C17" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">16. </v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="12">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C18" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">17. </v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="12">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C19" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">18. </v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="12">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C20" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">19. </v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="12">
         <v>20</v>
+      </c>
+      <c r="C21" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">20. </v>
       </c>
     </row>
   </sheetData>
@@ -788,15 +884,15 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B16" sqref="B16"/>
-      <selection pane="bottomLeft" sqref="A1:C1048576"/>
+      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="12"/>
-    <col min="2" max="3" width="52.6640625" style="4" customWidth="1"/>
+    <col min="2" max="3" width="53" style="4" customWidth="1"/>
     <col min="4" max="16384" width="8.88671875" style="8"/>
   </cols>
   <sheetData>
@@ -811,7 +907,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="12">
         <v>1</v>
       </c>
@@ -822,7 +918,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A3" s="12">
         <v>2</v>
       </c>
@@ -975,10 +1071,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB05837C-FA7D-4C9E-B312-A520296196E1}">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B16" sqref="B16"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1:C1048576"/>
+      <selection pane="bottomLeft" activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>